<commit_message>
filtri funzionanti, TODO: re-render scatter
</commit_message>
<xml_diff>
--- a/datasets/december.xlsx
+++ b/datasets/december.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documents\GitHub\VisualAnalytics\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3D1C65-C038-410C-B6E9-B5B45EB5E944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A00531-7DF2-42DA-ABEF-9C2CA9CFDC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6362" uniqueCount="2441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6609" uniqueCount="2442">
   <si>
     <t>s.no</t>
   </si>
@@ -7343,6 +7343,9 @@
   </si>
   <si>
     <t>MrBeast6000</t>
+  </si>
+  <si>
+    <t>Mixed</t>
   </si>
 </sst>
 </file>
@@ -8186,7 +8189,7 @@
   <dimension ref="A1:J827"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8268,6 +8271,9 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
+      <c r="D3" t="s">
+        <v>2441</v>
+      </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
@@ -8457,6 +8463,9 @@
       <c r="C9" t="s">
         <v>56</v>
       </c>
+      <c r="D9" t="s">
+        <v>2441</v>
+      </c>
       <c r="E9" t="s">
         <v>57</v>
       </c>
@@ -8486,6 +8495,9 @@
       <c r="C10" t="s">
         <v>59</v>
       </c>
+      <c r="D10" t="s">
+        <v>2441</v>
+      </c>
       <c r="E10" t="s">
         <v>60</v>
       </c>
@@ -8643,6 +8655,9 @@
       <c r="C15" t="s">
         <v>85</v>
       </c>
+      <c r="D15" t="s">
+        <v>2441</v>
+      </c>
       <c r="E15" t="s">
         <v>86</v>
       </c>
@@ -8768,6 +8783,9 @@
       <c r="C19" t="s">
         <v>103</v>
       </c>
+      <c r="D19" t="s">
+        <v>2441</v>
+      </c>
       <c r="E19" t="s">
         <v>104</v>
       </c>
@@ -9117,6 +9135,9 @@
       <c r="C30" t="s">
         <v>152</v>
       </c>
+      <c r="D30" t="s">
+        <v>2441</v>
+      </c>
       <c r="E30" t="s">
         <v>153</v>
       </c>
@@ -9146,6 +9167,9 @@
       <c r="C31" t="s">
         <v>156</v>
       </c>
+      <c r="D31" t="s">
+        <v>2441</v>
+      </c>
       <c r="E31" t="s">
         <v>157</v>
       </c>
@@ -9207,6 +9231,9 @@
       <c r="C33" t="s">
         <v>165</v>
       </c>
+      <c r="D33" t="s">
+        <v>2441</v>
+      </c>
       <c r="E33" t="s">
         <v>166</v>
       </c>
@@ -9332,6 +9359,9 @@
       <c r="C37" t="s">
         <v>187</v>
       </c>
+      <c r="D37" t="s">
+        <v>2441</v>
+      </c>
       <c r="E37" t="s">
         <v>188</v>
       </c>
@@ -9361,6 +9391,9 @@
       <c r="C38" t="s">
         <v>191</v>
       </c>
+      <c r="D38" t="s">
+        <v>2441</v>
+      </c>
       <c r="E38" t="s">
         <v>192</v>
       </c>
@@ -9422,6 +9455,9 @@
       <c r="C40" t="s">
         <v>201</v>
       </c>
+      <c r="D40" t="s">
+        <v>2441</v>
+      </c>
       <c r="E40" t="s">
         <v>202</v>
       </c>
@@ -9451,6 +9487,9 @@
       <c r="C41" t="s">
         <v>208</v>
       </c>
+      <c r="D41" t="s">
+        <v>2441</v>
+      </c>
       <c r="E41" t="s">
         <v>209</v>
       </c>
@@ -9576,6 +9615,9 @@
       <c r="C45" t="s">
         <v>228</v>
       </c>
+      <c r="D45" t="s">
+        <v>2441</v>
+      </c>
       <c r="E45" t="s">
         <v>229</v>
       </c>
@@ -9669,6 +9711,9 @@
       <c r="C48" t="s">
         <v>242</v>
       </c>
+      <c r="D48" t="s">
+        <v>2441</v>
+      </c>
       <c r="E48" t="s">
         <v>243</v>
       </c>
@@ -9698,6 +9743,9 @@
       <c r="C49" t="s">
         <v>247</v>
       </c>
+      <c r="D49" t="s">
+        <v>2441</v>
+      </c>
       <c r="E49" t="s">
         <v>248</v>
       </c>
@@ -9791,6 +9839,9 @@
       <c r="C52" t="s">
         <v>261</v>
       </c>
+      <c r="D52" t="s">
+        <v>2441</v>
+      </c>
       <c r="E52" t="s">
         <v>262</v>
       </c>
@@ -9852,6 +9903,9 @@
       <c r="C54" t="s">
         <v>271</v>
       </c>
+      <c r="D54" t="s">
+        <v>2441</v>
+      </c>
       <c r="E54" t="s">
         <v>269</v>
       </c>
@@ -9977,6 +10031,9 @@
       <c r="C58" t="s">
         <v>285</v>
       </c>
+      <c r="D58" t="s">
+        <v>2441</v>
+      </c>
       <c r="E58" t="s">
         <v>286</v>
       </c>
@@ -10006,6 +10063,9 @@
       <c r="C59" t="s">
         <v>289</v>
       </c>
+      <c r="D59" t="s">
+        <v>2441</v>
+      </c>
       <c r="E59" t="s">
         <v>290</v>
       </c>
@@ -10035,6 +10095,9 @@
       <c r="C60" t="s">
         <v>293</v>
       </c>
+      <c r="D60" t="s">
+        <v>2441</v>
+      </c>
       <c r="E60" t="s">
         <v>290</v>
       </c>
@@ -10096,6 +10159,9 @@
       <c r="C62" t="s">
         <v>302</v>
       </c>
+      <c r="D62" t="s">
+        <v>2441</v>
+      </c>
       <c r="E62" t="s">
         <v>299</v>
       </c>
@@ -10125,6 +10191,9 @@
       <c r="C63" t="s">
         <v>304</v>
       </c>
+      <c r="D63" t="s">
+        <v>2441</v>
+      </c>
       <c r="E63" t="s">
         <v>305</v>
       </c>
@@ -10154,6 +10223,9 @@
       <c r="C64" t="s">
         <v>308</v>
       </c>
+      <c r="D64" t="s">
+        <v>2441</v>
+      </c>
       <c r="E64" t="s">
         <v>309</v>
       </c>
@@ -10407,6 +10479,9 @@
       <c r="C72" t="s">
         <v>337</v>
       </c>
+      <c r="D72" t="s">
+        <v>2441</v>
+      </c>
       <c r="E72" t="s">
         <v>338</v>
       </c>
@@ -10436,6 +10511,9 @@
       <c r="C73" t="s">
         <v>341</v>
       </c>
+      <c r="D73" t="s">
+        <v>2441</v>
+      </c>
       <c r="E73" t="s">
         <v>342</v>
       </c>
@@ -10465,6 +10543,9 @@
       <c r="C74" t="s">
         <v>345</v>
       </c>
+      <c r="D74" t="s">
+        <v>2441</v>
+      </c>
       <c r="E74" t="s">
         <v>346</v>
       </c>
@@ -10526,6 +10607,9 @@
       <c r="C76" t="s">
         <v>355</v>
       </c>
+      <c r="D76" t="s">
+        <v>2441</v>
+      </c>
       <c r="E76" t="s">
         <v>351</v>
       </c>
@@ -10619,6 +10703,9 @@
       <c r="C79" t="s">
         <v>365</v>
       </c>
+      <c r="D79" t="s">
+        <v>2441</v>
+      </c>
       <c r="E79" t="s">
         <v>366</v>
       </c>
@@ -10680,6 +10767,9 @@
       <c r="C81" t="s">
         <v>372</v>
       </c>
+      <c r="D81" t="s">
+        <v>2441</v>
+      </c>
       <c r="E81" t="s">
         <v>373</v>
       </c>
@@ -10933,6 +11023,9 @@
       <c r="C89" t="s">
         <v>403</v>
       </c>
+      <c r="D89" t="s">
+        <v>2441</v>
+      </c>
       <c r="E89" t="s">
         <v>404</v>
       </c>
@@ -11058,6 +11151,9 @@
       <c r="C93" t="s">
         <v>420</v>
       </c>
+      <c r="D93" t="s">
+        <v>2441</v>
+      </c>
       <c r="E93" t="s">
         <v>421</v>
       </c>
@@ -11183,6 +11279,9 @@
       <c r="C97" t="s">
         <v>440</v>
       </c>
+      <c r="D97" t="s">
+        <v>2441</v>
+      </c>
       <c r="E97" t="s">
         <v>437</v>
       </c>
@@ -11212,6 +11311,9 @@
       <c r="C98" t="s">
         <v>442</v>
       </c>
+      <c r="D98" t="s">
+        <v>2441</v>
+      </c>
       <c r="E98" t="s">
         <v>437</v>
       </c>
@@ -11273,6 +11375,9 @@
       <c r="C100" t="s">
         <v>451</v>
       </c>
+      <c r="D100" t="s">
+        <v>2441</v>
+      </c>
       <c r="E100" t="s">
         <v>452</v>
       </c>
@@ -11398,6 +11503,9 @@
       <c r="C104" t="s">
         <v>468</v>
       </c>
+      <c r="D104" t="s">
+        <v>2441</v>
+      </c>
       <c r="E104" t="s">
         <v>465</v>
       </c>
@@ -11555,6 +11663,9 @@
       <c r="C109" t="s">
         <v>492</v>
       </c>
+      <c r="D109" t="s">
+        <v>2441</v>
+      </c>
       <c r="E109" t="s">
         <v>490</v>
       </c>
@@ -11776,6 +11887,9 @@
       <c r="C116" t="s">
         <v>522</v>
       </c>
+      <c r="D116" t="s">
+        <v>2441</v>
+      </c>
       <c r="E116" t="s">
         <v>523</v>
       </c>
@@ -11837,6 +11951,9 @@
       <c r="C118" t="s">
         <v>528</v>
       </c>
+      <c r="D118" t="s">
+        <v>2441</v>
+      </c>
       <c r="E118" t="s">
         <v>529</v>
       </c>
@@ -11898,6 +12015,9 @@
       <c r="C120" t="s">
         <v>537</v>
       </c>
+      <c r="D120" t="s">
+        <v>2441</v>
+      </c>
       <c r="E120" t="s">
         <v>533</v>
       </c>
@@ -12119,6 +12239,9 @@
       <c r="C127" t="s">
         <v>561</v>
       </c>
+      <c r="D127" t="s">
+        <v>2441</v>
+      </c>
       <c r="E127" t="s">
         <v>562</v>
       </c>
@@ -12212,6 +12335,9 @@
       <c r="C130" t="s">
         <v>573</v>
       </c>
+      <c r="D130" t="s">
+        <v>2441</v>
+      </c>
       <c r="E130" t="s">
         <v>280</v>
       </c>
@@ -12305,6 +12431,9 @@
       <c r="C133" t="s">
         <v>585</v>
       </c>
+      <c r="D133" t="s">
+        <v>2441</v>
+      </c>
       <c r="E133" t="s">
         <v>586</v>
       </c>
@@ -12494,6 +12623,9 @@
       <c r="C139" t="s">
         <v>613</v>
       </c>
+      <c r="D139" t="s">
+        <v>2441</v>
+      </c>
       <c r="E139" t="s">
         <v>614</v>
       </c>
@@ -12619,6 +12751,9 @@
       <c r="C143" t="s">
         <v>628</v>
       </c>
+      <c r="D143" t="s">
+        <v>2441</v>
+      </c>
       <c r="E143" t="s">
         <v>629</v>
       </c>
@@ -12808,6 +12943,9 @@
       <c r="C149" t="s">
         <v>651</v>
       </c>
+      <c r="D149" t="s">
+        <v>2441</v>
+      </c>
       <c r="E149" t="s">
         <v>649</v>
       </c>
@@ -12965,6 +13103,9 @@
       <c r="C154" t="s">
         <v>666</v>
       </c>
+      <c r="D154" t="s">
+        <v>2441</v>
+      </c>
       <c r="E154" t="s">
         <v>662</v>
       </c>
@@ -13026,6 +13167,9 @@
       <c r="C156" t="s">
         <v>678</v>
       </c>
+      <c r="D156" t="s">
+        <v>2441</v>
+      </c>
       <c r="E156" t="s">
         <v>679</v>
       </c>
@@ -13087,6 +13231,9 @@
       <c r="C158" t="s">
         <v>685</v>
       </c>
+      <c r="D158" t="s">
+        <v>2441</v>
+      </c>
       <c r="E158" t="s">
         <v>682</v>
       </c>
@@ -13148,6 +13295,9 @@
       <c r="C160" t="s">
         <v>691</v>
       </c>
+      <c r="D160" t="s">
+        <v>2441</v>
+      </c>
       <c r="E160" t="s">
         <v>682</v>
       </c>
@@ -13209,6 +13359,9 @@
       <c r="C162" t="s">
         <v>699</v>
       </c>
+      <c r="D162" t="s">
+        <v>2441</v>
+      </c>
       <c r="E162" t="s">
         <v>697</v>
       </c>
@@ -13238,6 +13391,9 @@
       <c r="C163" t="s">
         <v>700</v>
       </c>
+      <c r="D163" t="s">
+        <v>2441</v>
+      </c>
       <c r="E163" t="s">
         <v>697</v>
       </c>
@@ -13267,6 +13423,9 @@
       <c r="C164" t="s">
         <v>702</v>
       </c>
+      <c r="D164" t="s">
+        <v>2441</v>
+      </c>
       <c r="E164" t="s">
         <v>697</v>
       </c>
@@ -13520,6 +13679,9 @@
       <c r="C172" t="s">
         <v>728</v>
       </c>
+      <c r="D172" t="s">
+        <v>2441</v>
+      </c>
       <c r="E172" t="s">
         <v>729</v>
       </c>
@@ -13677,6 +13839,9 @@
       <c r="C177" t="s">
         <v>747</v>
       </c>
+      <c r="D177" t="s">
+        <v>2441</v>
+      </c>
       <c r="E177" t="s">
         <v>746</v>
       </c>
@@ -13802,6 +13967,9 @@
       <c r="C181" t="s">
         <v>760</v>
       </c>
+      <c r="D181" t="s">
+        <v>2441</v>
+      </c>
       <c r="E181" t="s">
         <v>761</v>
       </c>
@@ -13831,6 +13999,9 @@
       <c r="C182" t="s">
         <v>764</v>
       </c>
+      <c r="D182" t="s">
+        <v>2441</v>
+      </c>
       <c r="E182" t="s">
         <v>761</v>
       </c>
@@ -13956,6 +14127,9 @@
       <c r="C186" t="s">
         <v>777</v>
       </c>
+      <c r="D186" t="s">
+        <v>2441</v>
+      </c>
       <c r="E186" t="s">
         <v>778</v>
       </c>
@@ -13985,6 +14159,9 @@
       <c r="C187" t="s">
         <v>780</v>
       </c>
+      <c r="D187" t="s">
+        <v>2441</v>
+      </c>
       <c r="E187" t="s">
         <v>778</v>
       </c>
@@ -14046,6 +14223,9 @@
       <c r="C189" t="s">
         <v>786</v>
       </c>
+      <c r="D189" t="s">
+        <v>2441</v>
+      </c>
       <c r="E189" t="s">
         <v>784</v>
       </c>
@@ -14171,6 +14351,9 @@
       <c r="C193" t="s">
         <v>798</v>
       </c>
+      <c r="D193" t="s">
+        <v>2441</v>
+      </c>
       <c r="E193" t="s">
         <v>794</v>
       </c>
@@ -14296,6 +14479,9 @@
       <c r="C197" t="s">
         <v>811</v>
       </c>
+      <c r="D197" t="s">
+        <v>2441</v>
+      </c>
       <c r="E197" t="s">
         <v>804</v>
       </c>
@@ -14389,6 +14575,9 @@
       <c r="C200" t="s">
         <v>821</v>
       </c>
+      <c r="D200" t="s">
+        <v>2441</v>
+      </c>
       <c r="E200" t="s">
         <v>817</v>
       </c>
@@ -14482,6 +14671,9 @@
       <c r="C203" t="s">
         <v>828</v>
       </c>
+      <c r="D203" t="s">
+        <v>2441</v>
+      </c>
       <c r="E203" t="s">
         <v>829</v>
       </c>
@@ -14639,6 +14831,9 @@
       <c r="C208" t="s">
         <v>844</v>
       </c>
+      <c r="D208" t="s">
+        <v>2441</v>
+      </c>
       <c r="E208" t="s">
         <v>835</v>
       </c>
@@ -14732,6 +14927,9 @@
       <c r="C211" t="s">
         <v>855</v>
       </c>
+      <c r="D211" t="s">
+        <v>2441</v>
+      </c>
       <c r="E211" t="s">
         <v>856</v>
       </c>
@@ -14793,6 +14991,9 @@
       <c r="C213" t="s">
         <v>862</v>
       </c>
+      <c r="D213" t="s">
+        <v>2441</v>
+      </c>
       <c r="E213" t="s">
         <v>856</v>
       </c>
@@ -14886,6 +15087,9 @@
       <c r="C216" t="s">
         <v>870</v>
       </c>
+      <c r="D216" t="s">
+        <v>2441</v>
+      </c>
       <c r="E216" t="s">
         <v>871</v>
       </c>
@@ -15075,6 +15279,9 @@
       <c r="C222" t="s">
         <v>891</v>
       </c>
+      <c r="D222" t="s">
+        <v>2441</v>
+      </c>
       <c r="E222" t="s">
         <v>892</v>
       </c>
@@ -15232,6 +15439,9 @@
       <c r="C227" t="s">
         <v>911</v>
       </c>
+      <c r="D227" t="s">
+        <v>2441</v>
+      </c>
       <c r="E227" t="s">
         <v>910</v>
       </c>
@@ -15325,6 +15535,9 @@
       <c r="C230" t="s">
         <v>921</v>
       </c>
+      <c r="D230" t="s">
+        <v>2441</v>
+      </c>
       <c r="E230" t="s">
         <v>918</v>
       </c>
@@ -15354,6 +15567,9 @@
       <c r="C231" t="s">
         <v>923</v>
       </c>
+      <c r="D231" t="s">
+        <v>2441</v>
+      </c>
       <c r="E231" t="s">
         <v>918</v>
       </c>
@@ -15511,6 +15727,9 @@
       <c r="C236" t="s">
         <v>941</v>
       </c>
+      <c r="D236" t="s">
+        <v>2441</v>
+      </c>
       <c r="E236" t="s">
         <v>937</v>
       </c>
@@ -15668,6 +15887,9 @@
       <c r="C241" t="s">
         <v>956</v>
       </c>
+      <c r="D241" t="s">
+        <v>2441</v>
+      </c>
       <c r="E241" t="s">
         <v>957</v>
       </c>
@@ -15729,6 +15951,9 @@
       <c r="C243" t="s">
         <v>963</v>
       </c>
+      <c r="D243" t="s">
+        <v>2441</v>
+      </c>
       <c r="E243" t="s">
         <v>957</v>
       </c>
@@ -15822,6 +16047,9 @@
       <c r="C246" t="s">
         <v>974</v>
       </c>
+      <c r="D246" t="s">
+        <v>2441</v>
+      </c>
       <c r="E246" t="s">
         <v>957</v>
       </c>
@@ -16075,6 +16303,9 @@
       <c r="C254" t="s">
         <v>999</v>
       </c>
+      <c r="D254" t="s">
+        <v>2441</v>
+      </c>
       <c r="E254" t="s">
         <v>995</v>
       </c>
@@ -16136,6 +16367,9 @@
       <c r="C256" t="s">
         <v>1005</v>
       </c>
+      <c r="D256" t="s">
+        <v>2441</v>
+      </c>
       <c r="E256" t="s">
         <v>1006</v>
       </c>
@@ -16197,6 +16431,9 @@
       <c r="C258" t="s">
         <v>1012</v>
       </c>
+      <c r="D258" t="s">
+        <v>2441</v>
+      </c>
       <c r="E258" t="s">
         <v>1009</v>
       </c>
@@ -16546,6 +16783,9 @@
       <c r="C269" t="s">
         <v>1045</v>
       </c>
+      <c r="D269" t="s">
+        <v>2441</v>
+      </c>
       <c r="E269" t="s">
         <v>1046</v>
       </c>
@@ -16639,6 +16879,9 @@
       <c r="C272" t="s">
         <v>1054</v>
       </c>
+      <c r="D272" t="s">
+        <v>2441</v>
+      </c>
       <c r="E272" t="s">
         <v>1046</v>
       </c>
@@ -16764,6 +17007,9 @@
       <c r="C276" t="s">
         <v>1069</v>
       </c>
+      <c r="D276" t="s">
+        <v>2441</v>
+      </c>
       <c r="E276" t="s">
         <v>1065</v>
       </c>
@@ -16793,6 +17039,9 @@
       <c r="C277" t="s">
         <v>1072</v>
       </c>
+      <c r="D277" t="s">
+        <v>2441</v>
+      </c>
       <c r="E277" t="s">
         <v>1065</v>
       </c>
@@ -16886,6 +17135,9 @@
       <c r="C280" t="s">
         <v>1084</v>
       </c>
+      <c r="D280" t="s">
+        <v>2441</v>
+      </c>
       <c r="E280" t="s">
         <v>1079</v>
       </c>
@@ -17011,6 +17263,9 @@
       <c r="C284" t="s">
         <v>1102</v>
       </c>
+      <c r="D284" t="s">
+        <v>2441</v>
+      </c>
       <c r="E284" t="s">
         <v>1090</v>
       </c>
@@ -17104,6 +17359,9 @@
       <c r="C287" t="s">
         <v>1111</v>
       </c>
+      <c r="D287" t="s">
+        <v>2441</v>
+      </c>
       <c r="E287" t="s">
         <v>1105</v>
       </c>
@@ -17133,6 +17391,9 @@
       <c r="C288" t="s">
         <v>1113</v>
       </c>
+      <c r="D288" t="s">
+        <v>2441</v>
+      </c>
       <c r="E288" t="s">
         <v>1105</v>
       </c>
@@ -17258,6 +17519,9 @@
       <c r="C292" t="s">
         <v>1125</v>
       </c>
+      <c r="D292" t="s">
+        <v>2441</v>
+      </c>
       <c r="E292" t="s">
         <v>1123</v>
       </c>
@@ -17319,6 +17583,9 @@
       <c r="C294" t="s">
         <v>1131</v>
       </c>
+      <c r="D294" t="s">
+        <v>2441</v>
+      </c>
       <c r="E294" t="s">
         <v>1123</v>
       </c>
@@ -17508,6 +17775,9 @@
       <c r="C300" t="s">
         <v>1151</v>
       </c>
+      <c r="D300" t="s">
+        <v>2441</v>
+      </c>
       <c r="E300" t="s">
         <v>1145</v>
       </c>
@@ -17537,6 +17807,9 @@
       <c r="C301" t="s">
         <v>1153</v>
       </c>
+      <c r="D301" t="s">
+        <v>2441</v>
+      </c>
       <c r="E301" t="s">
         <v>1154</v>
       </c>
@@ -17598,6 +17871,9 @@
       <c r="C303" t="s">
         <v>1159</v>
       </c>
+      <c r="D303" t="s">
+        <v>2441</v>
+      </c>
       <c r="E303" t="s">
         <v>1154</v>
       </c>
@@ -17723,6 +17999,9 @@
       <c r="C307" t="s">
         <v>1172</v>
       </c>
+      <c r="D307" t="s">
+        <v>2441</v>
+      </c>
       <c r="E307" t="s">
         <v>1161</v>
       </c>
@@ -17880,6 +18159,9 @@
       <c r="C312" t="s">
         <v>1187</v>
       </c>
+      <c r="D312" t="s">
+        <v>2441</v>
+      </c>
       <c r="E312" t="s">
         <v>1179</v>
       </c>
@@ -17909,6 +18191,9 @@
       <c r="C313" t="s">
         <v>1188</v>
       </c>
+      <c r="D313" t="s">
+        <v>2441</v>
+      </c>
       <c r="E313" t="s">
         <v>1179</v>
       </c>
@@ -18066,6 +18351,9 @@
       <c r="C318" t="s">
         <v>1200</v>
       </c>
+      <c r="D318" t="s">
+        <v>2441</v>
+      </c>
       <c r="E318" t="s">
         <v>1201</v>
       </c>
@@ -18159,6 +18447,9 @@
       <c r="C321" t="s">
         <v>1206</v>
       </c>
+      <c r="D321" t="s">
+        <v>2441</v>
+      </c>
       <c r="E321" t="s">
         <v>1201</v>
       </c>
@@ -18252,6 +18543,9 @@
       <c r="C324" t="s">
         <v>1216</v>
       </c>
+      <c r="D324" t="s">
+        <v>2441</v>
+      </c>
       <c r="E324" t="s">
         <v>1213</v>
       </c>
@@ -18409,6 +18703,9 @@
       <c r="C329" t="s">
         <v>1231</v>
       </c>
+      <c r="D329" t="s">
+        <v>2441</v>
+      </c>
       <c r="E329" t="s">
         <v>1218</v>
       </c>
@@ -18534,6 +18831,9 @@
       <c r="C333" t="s">
         <v>1242</v>
       </c>
+      <c r="D333" t="s">
+        <v>2441</v>
+      </c>
       <c r="E333" t="s">
         <v>1237</v>
       </c>
@@ -18691,6 +18991,9 @@
       <c r="C338" t="s">
         <v>1252</v>
       </c>
+      <c r="D338" t="s">
+        <v>2441</v>
+      </c>
       <c r="E338" t="s">
         <v>1249</v>
       </c>
@@ -18752,6 +19055,9 @@
       <c r="C340" t="s">
         <v>1256</v>
       </c>
+      <c r="D340" t="s">
+        <v>2441</v>
+      </c>
       <c r="E340" t="s">
         <v>1257</v>
       </c>
@@ -18813,6 +19119,9 @@
       <c r="C342" t="s">
         <v>1260</v>
       </c>
+      <c r="D342" t="s">
+        <v>2441</v>
+      </c>
       <c r="E342" t="s">
         <v>1257</v>
       </c>
@@ -18970,6 +19279,9 @@
       <c r="C347" t="s">
         <v>1277</v>
       </c>
+      <c r="D347" t="s">
+        <v>2441</v>
+      </c>
       <c r="E347" t="s">
         <v>1275</v>
       </c>
@@ -19031,6 +19343,9 @@
       <c r="C349" t="s">
         <v>1280</v>
       </c>
+      <c r="D349" t="s">
+        <v>2441</v>
+      </c>
       <c r="E349" t="s">
         <v>1275</v>
       </c>
@@ -19220,6 +19535,9 @@
       <c r="C355" t="s">
         <v>1295</v>
       </c>
+      <c r="D355" t="s">
+        <v>2441</v>
+      </c>
       <c r="E355" t="s">
         <v>1286</v>
       </c>
@@ -19313,6 +19631,9 @@
       <c r="C358" t="s">
         <v>1302</v>
       </c>
+      <c r="D358" t="s">
+        <v>2441</v>
+      </c>
       <c r="E358" t="s">
         <v>1301</v>
       </c>
@@ -19342,6 +19663,9 @@
       <c r="C359" t="s">
         <v>1304</v>
       </c>
+      <c r="D359" t="s">
+        <v>2441</v>
+      </c>
       <c r="E359" t="s">
         <v>1301</v>
       </c>
@@ -19371,6 +19695,9 @@
       <c r="C360" t="s">
         <v>1307</v>
       </c>
+      <c r="D360" t="s">
+        <v>2441</v>
+      </c>
       <c r="E360" t="s">
         <v>1301</v>
       </c>
@@ -19496,6 +19823,9 @@
       <c r="C364" t="s">
         <v>1314</v>
       </c>
+      <c r="D364" t="s">
+        <v>2441</v>
+      </c>
       <c r="E364" t="s">
         <v>1301</v>
       </c>
@@ -19653,6 +19983,9 @@
       <c r="C369" t="s">
         <v>1331</v>
       </c>
+      <c r="D369" t="s">
+        <v>2441</v>
+      </c>
       <c r="E369" t="s">
         <v>1327</v>
       </c>
@@ -19938,6 +20271,9 @@
       <c r="C378" t="s">
         <v>1357</v>
       </c>
+      <c r="D378" t="s">
+        <v>2441</v>
+      </c>
       <c r="E378" t="s">
         <v>1352</v>
       </c>
@@ -20063,6 +20399,9 @@
       <c r="C382" t="s">
         <v>1368</v>
       </c>
+      <c r="D382" t="s">
+        <v>2441</v>
+      </c>
       <c r="E382" t="s">
         <v>1369</v>
       </c>
@@ -20444,6 +20783,9 @@
       <c r="C394" t="s">
         <v>1398</v>
       </c>
+      <c r="D394" t="s">
+        <v>2441</v>
+      </c>
       <c r="E394" t="s">
         <v>254</v>
       </c>
@@ -20473,6 +20815,9 @@
       <c r="C395" t="s">
         <v>1400</v>
       </c>
+      <c r="D395" t="s">
+        <v>2441</v>
+      </c>
       <c r="E395" t="s">
         <v>1401</v>
       </c>
@@ -20502,6 +20847,9 @@
       <c r="C396" t="s">
         <v>1403</v>
       </c>
+      <c r="D396" t="s">
+        <v>2441</v>
+      </c>
       <c r="E396" t="s">
         <v>1401</v>
       </c>
@@ -20531,6 +20879,9 @@
       <c r="C397" t="s">
         <v>1405</v>
       </c>
+      <c r="D397" t="s">
+        <v>2441</v>
+      </c>
       <c r="E397" t="s">
         <v>1401</v>
       </c>
@@ -20656,6 +21007,9 @@
       <c r="C401" t="s">
         <v>1416</v>
       </c>
+      <c r="D401" t="s">
+        <v>2441</v>
+      </c>
       <c r="E401" t="s">
         <v>1401</v>
       </c>
@@ -20685,6 +21039,9 @@
       <c r="C402" t="s">
         <v>1417</v>
       </c>
+      <c r="D402" t="s">
+        <v>2441</v>
+      </c>
       <c r="E402" t="s">
         <v>1401</v>
       </c>
@@ -20874,6 +21231,9 @@
       <c r="C408" t="s">
         <v>1429</v>
       </c>
+      <c r="D408" t="s">
+        <v>2441</v>
+      </c>
       <c r="E408" t="s">
         <v>272</v>
       </c>
@@ -20903,6 +21263,9 @@
       <c r="C409" t="s">
         <v>1431</v>
       </c>
+      <c r="D409" t="s">
+        <v>2441</v>
+      </c>
       <c r="E409" t="s">
         <v>272</v>
       </c>
@@ -20964,6 +21327,9 @@
       <c r="C411" t="s">
         <v>1435</v>
       </c>
+      <c r="D411" t="s">
+        <v>2441</v>
+      </c>
       <c r="E411" t="s">
         <v>1436</v>
       </c>
@@ -20993,6 +21359,9 @@
       <c r="C412" t="s">
         <v>1438</v>
       </c>
+      <c r="D412" t="s">
+        <v>2441</v>
+      </c>
       <c r="E412" t="s">
         <v>1436</v>
       </c>
@@ -21086,6 +21455,9 @@
       <c r="C415" t="s">
         <v>1445</v>
       </c>
+      <c r="D415" t="s">
+        <v>2441</v>
+      </c>
       <c r="E415" t="s">
         <v>1436</v>
       </c>
@@ -21147,6 +21519,9 @@
       <c r="C417" t="s">
         <v>1450</v>
       </c>
+      <c r="D417" t="s">
+        <v>2441</v>
+      </c>
       <c r="E417" t="s">
         <v>1436</v>
       </c>
@@ -21176,6 +21551,9 @@
       <c r="C418" t="s">
         <v>1452</v>
       </c>
+      <c r="D418" t="s">
+        <v>2441</v>
+      </c>
       <c r="E418" t="s">
         <v>1436</v>
       </c>
@@ -21493,6 +21871,9 @@
       <c r="C428" t="s">
         <v>1483</v>
       </c>
+      <c r="D428" t="s">
+        <v>2441</v>
+      </c>
       <c r="E428" t="s">
         <v>1460</v>
       </c>
@@ -21650,6 +22031,9 @@
       <c r="C433" t="s">
         <v>1495</v>
       </c>
+      <c r="D433" t="s">
+        <v>2441</v>
+      </c>
       <c r="E433" t="s">
         <v>1496</v>
       </c>
@@ -21807,6 +22191,9 @@
       <c r="C438" t="s">
         <v>1509</v>
       </c>
+      <c r="D438" t="s">
+        <v>2441</v>
+      </c>
       <c r="E438" t="s">
         <v>1506</v>
       </c>
@@ -21964,6 +22351,9 @@
       <c r="C443" t="s">
         <v>1525</v>
       </c>
+      <c r="D443" t="s">
+        <v>2441</v>
+      </c>
       <c r="E443" t="s">
         <v>1526</v>
       </c>
@@ -22025,6 +22415,9 @@
       <c r="C445" t="s">
         <v>1529</v>
       </c>
+      <c r="D445" t="s">
+        <v>2441</v>
+      </c>
       <c r="E445" t="s">
         <v>1526</v>
       </c>
@@ -22054,6 +22447,9 @@
       <c r="C446" t="s">
         <v>1532</v>
       </c>
+      <c r="D446" t="s">
+        <v>2441</v>
+      </c>
       <c r="E446" t="s">
         <v>1526</v>
       </c>
@@ -22307,6 +22703,9 @@
       <c r="C454" t="s">
         <v>1555</v>
       </c>
+      <c r="D454" t="s">
+        <v>2441</v>
+      </c>
       <c r="E454" t="s">
         <v>1545</v>
       </c>
@@ -22368,6 +22767,9 @@
       <c r="C456" t="s">
         <v>1559</v>
       </c>
+      <c r="D456" t="s">
+        <v>2441</v>
+      </c>
       <c r="E456" t="s">
         <v>1558</v>
       </c>
@@ -22557,6 +22959,9 @@
       <c r="C462" t="s">
         <v>1574</v>
       </c>
+      <c r="D462" t="s">
+        <v>2441</v>
+      </c>
       <c r="E462" t="s">
         <v>1558</v>
       </c>
@@ -22618,6 +23023,9 @@
       <c r="C464" t="s">
         <v>1580</v>
       </c>
+      <c r="D464" t="s">
+        <v>2441</v>
+      </c>
       <c r="E464" t="s">
         <v>1578</v>
       </c>
@@ -22647,6 +23055,9 @@
       <c r="C465" t="s">
         <v>1582</v>
       </c>
+      <c r="D465" t="s">
+        <v>2441</v>
+      </c>
       <c r="E465" t="s">
         <v>1578</v>
       </c>
@@ -22868,6 +23279,9 @@
       <c r="C472" t="s">
         <v>1600</v>
       </c>
+      <c r="D472" t="s">
+        <v>2441</v>
+      </c>
       <c r="E472" t="s">
         <v>1592</v>
       </c>
@@ -22897,6 +23311,9 @@
       <c r="C473" t="s">
         <v>1601</v>
       </c>
+      <c r="D473" t="s">
+        <v>2441</v>
+      </c>
       <c r="E473" t="s">
         <v>1592</v>
       </c>
@@ -23150,6 +23567,9 @@
       <c r="C481" t="s">
         <v>1619</v>
       </c>
+      <c r="D481" t="s">
+        <v>2441</v>
+      </c>
       <c r="E481" t="s">
         <v>1614</v>
       </c>
@@ -23307,6 +23727,9 @@
       <c r="C486" t="s">
         <v>1630</v>
       </c>
+      <c r="D486" t="s">
+        <v>2441</v>
+      </c>
       <c r="E486" t="s">
         <v>1631</v>
       </c>
@@ -23464,6 +23887,9 @@
       <c r="C491" t="s">
         <v>1644</v>
       </c>
+      <c r="D491" t="s">
+        <v>2441</v>
+      </c>
       <c r="E491" t="s">
         <v>1631</v>
       </c>
@@ -23717,6 +24143,9 @@
       <c r="C499" t="s">
         <v>1669</v>
       </c>
+      <c r="D499" t="s">
+        <v>2441</v>
+      </c>
       <c r="E499" t="s">
         <v>1670</v>
       </c>
@@ -23746,6 +24175,9 @@
       <c r="C500" t="s">
         <v>1671</v>
       </c>
+      <c r="D500" t="s">
+        <v>2441</v>
+      </c>
       <c r="E500" t="s">
         <v>1670</v>
       </c>
@@ -24095,6 +24527,9 @@
       <c r="C511" t="s">
         <v>1699</v>
       </c>
+      <c r="D511" t="s">
+        <v>2441</v>
+      </c>
       <c r="E511" t="s">
         <v>1698</v>
       </c>
@@ -24220,6 +24655,9 @@
       <c r="C515" t="s">
         <v>1710</v>
       </c>
+      <c r="D515" t="s">
+        <v>2441</v>
+      </c>
       <c r="E515" t="s">
         <v>1698</v>
       </c>
@@ -24281,6 +24719,9 @@
       <c r="C517" t="s">
         <v>1714</v>
       </c>
+      <c r="D517" t="s">
+        <v>2441</v>
+      </c>
       <c r="E517" t="s">
         <v>1698</v>
       </c>
@@ -24406,6 +24847,9 @@
       <c r="C521" t="s">
         <v>1726</v>
       </c>
+      <c r="D521" t="s">
+        <v>2441</v>
+      </c>
       <c r="E521" t="s">
         <v>1723</v>
       </c>
@@ -24499,6 +24943,9 @@
       <c r="C524" t="s">
         <v>1731</v>
       </c>
+      <c r="D524" t="s">
+        <v>2441</v>
+      </c>
       <c r="E524" t="s">
         <v>1723</v>
       </c>
@@ -24560,6 +25007,9 @@
       <c r="C526" t="s">
         <v>1735</v>
       </c>
+      <c r="D526" t="s">
+        <v>2441</v>
+      </c>
       <c r="E526" t="s">
         <v>1736</v>
       </c>
@@ -24589,6 +25039,9 @@
       <c r="C527" t="s">
         <v>1739</v>
       </c>
+      <c r="D527" t="s">
+        <v>2441</v>
+      </c>
       <c r="E527" t="s">
         <v>1736</v>
       </c>
@@ -24650,6 +25103,9 @@
       <c r="C529" t="s">
         <v>1743</v>
       </c>
+      <c r="D529" t="s">
+        <v>2441</v>
+      </c>
       <c r="E529" t="s">
         <v>1736</v>
       </c>
@@ -24743,6 +25199,9 @@
       <c r="C532" t="s">
         <v>1748</v>
       </c>
+      <c r="D532" t="s">
+        <v>2441</v>
+      </c>
       <c r="E532" t="s">
         <v>1736</v>
       </c>
@@ -24804,6 +25263,9 @@
       <c r="C534" t="s">
         <v>1753</v>
       </c>
+      <c r="D534" t="s">
+        <v>2441</v>
+      </c>
       <c r="E534" t="s">
         <v>1736</v>
       </c>
@@ -24833,6 +25295,9 @@
       <c r="C535" t="s">
         <v>1754</v>
       </c>
+      <c r="D535" t="s">
+        <v>2441</v>
+      </c>
       <c r="E535" t="s">
         <v>1736</v>
       </c>
@@ -24926,6 +25391,9 @@
       <c r="C538" t="s">
         <v>1762</v>
       </c>
+      <c r="D538" t="s">
+        <v>2441</v>
+      </c>
       <c r="E538" t="s">
         <v>1757</v>
       </c>
@@ -24955,6 +25423,9 @@
       <c r="C539" t="s">
         <v>1765</v>
       </c>
+      <c r="D539" t="s">
+        <v>2441</v>
+      </c>
       <c r="E539" t="s">
         <v>1757</v>
       </c>
@@ -25272,6 +25743,9 @@
       <c r="C549" t="s">
         <v>1794</v>
       </c>
+      <c r="D549" t="s">
+        <v>2441</v>
+      </c>
       <c r="E549" t="s">
         <v>1791</v>
       </c>
@@ -25301,6 +25775,9 @@
       <c r="C550" t="s">
         <v>1796</v>
       </c>
+      <c r="D550" t="s">
+        <v>2441</v>
+      </c>
       <c r="E550" t="s">
         <v>1791</v>
       </c>
@@ -25330,6 +25807,9 @@
       <c r="C551" t="s">
         <v>1798</v>
       </c>
+      <c r="D551" t="s">
+        <v>2441</v>
+      </c>
       <c r="E551" t="s">
         <v>1791</v>
       </c>
@@ -25519,6 +25999,9 @@
       <c r="C557" t="s">
         <v>1812</v>
       </c>
+      <c r="D557" t="s">
+        <v>2441</v>
+      </c>
       <c r="E557" t="s">
         <v>1791</v>
       </c>
@@ -25580,6 +26063,9 @@
       <c r="C559" t="s">
         <v>1816</v>
       </c>
+      <c r="D559" t="s">
+        <v>2441</v>
+      </c>
       <c r="E559" t="s">
         <v>1791</v>
       </c>
@@ -25609,6 +26095,9 @@
       <c r="C560" t="s">
         <v>1819</v>
       </c>
+      <c r="D560" t="s">
+        <v>2441</v>
+      </c>
       <c r="E560" t="s">
         <v>1791</v>
       </c>
@@ -25766,6 +26255,9 @@
       <c r="C565" t="s">
         <v>1833</v>
       </c>
+      <c r="D565" t="s">
+        <v>2441</v>
+      </c>
       <c r="E565" t="s">
         <v>1828</v>
       </c>
@@ -25827,6 +26319,9 @@
       <c r="C567" t="s">
         <v>1838</v>
       </c>
+      <c r="D567" t="s">
+        <v>2441</v>
+      </c>
       <c r="E567" t="s">
         <v>1828</v>
       </c>
@@ -25920,6 +26415,9 @@
       <c r="C570" t="s">
         <v>1844</v>
       </c>
+      <c r="D570" t="s">
+        <v>2441</v>
+      </c>
       <c r="E570" t="s">
         <v>1845</v>
       </c>
@@ -25981,6 +26479,9 @@
       <c r="C572" t="s">
         <v>1850</v>
       </c>
+      <c r="D572" t="s">
+        <v>2441</v>
+      </c>
       <c r="E572" t="s">
         <v>1845</v>
       </c>
@@ -26074,6 +26575,9 @@
       <c r="C575" t="s">
         <v>1856</v>
       </c>
+      <c r="D575" t="s">
+        <v>2441</v>
+      </c>
       <c r="E575" t="s">
         <v>1845</v>
       </c>
@@ -26263,6 +26767,9 @@
       <c r="C581" t="s">
         <v>1869</v>
       </c>
+      <c r="D581" t="s">
+        <v>2441</v>
+      </c>
       <c r="E581" t="s">
         <v>1860</v>
       </c>
@@ -26420,6 +26927,9 @@
       <c r="C586" t="s">
         <v>1883</v>
       </c>
+      <c r="D586" t="s">
+        <v>2441</v>
+      </c>
       <c r="E586" t="s">
         <v>1879</v>
       </c>
@@ -26545,6 +27055,9 @@
       <c r="C590" t="s">
         <v>1892</v>
       </c>
+      <c r="D590" t="s">
+        <v>2441</v>
+      </c>
       <c r="E590" t="s">
         <v>1879</v>
       </c>
@@ -26862,6 +27375,9 @@
       <c r="C600" t="s">
         <v>1914</v>
       </c>
+      <c r="D600" t="s">
+        <v>2441</v>
+      </c>
       <c r="E600" t="s">
         <v>1080</v>
       </c>
@@ -26891,6 +27407,9 @@
       <c r="C601" t="s">
         <v>1915</v>
       </c>
+      <c r="D601" t="s">
+        <v>2441</v>
+      </c>
       <c r="E601" t="s">
         <v>1080</v>
       </c>
@@ -27016,6 +27535,9 @@
       <c r="C605" t="s">
         <v>1924</v>
       </c>
+      <c r="D605" t="s">
+        <v>2441</v>
+      </c>
       <c r="E605" t="s">
         <v>310</v>
       </c>
@@ -27045,6 +27567,9 @@
       <c r="C606" t="s">
         <v>1925</v>
       </c>
+      <c r="D606" t="s">
+        <v>2441</v>
+      </c>
       <c r="E606" t="s">
         <v>310</v>
       </c>
@@ -27074,6 +27599,9 @@
       <c r="C607" t="s">
         <v>1926</v>
       </c>
+      <c r="D607" t="s">
+        <v>2441</v>
+      </c>
       <c r="E607" t="s">
         <v>310</v>
       </c>
@@ -27199,6 +27727,9 @@
       <c r="C611" t="s">
         <v>1937</v>
       </c>
+      <c r="D611" t="s">
+        <v>2441</v>
+      </c>
       <c r="E611" t="s">
         <v>310</v>
       </c>
@@ -27260,6 +27791,9 @@
       <c r="C613" t="s">
         <v>1941</v>
       </c>
+      <c r="D613" t="s">
+        <v>2441</v>
+      </c>
       <c r="E613" t="s">
         <v>310</v>
       </c>
@@ -27321,6 +27855,9 @@
       <c r="C615" t="s">
         <v>1945</v>
       </c>
+      <c r="D615" t="s">
+        <v>2441</v>
+      </c>
       <c r="E615" t="s">
         <v>310</v>
       </c>
@@ -27414,6 +27951,9 @@
       <c r="C618" t="s">
         <v>1953</v>
       </c>
+      <c r="D618" t="s">
+        <v>2441</v>
+      </c>
       <c r="E618" t="s">
         <v>1951</v>
       </c>
@@ -27443,6 +27983,9 @@
       <c r="C619" t="s">
         <v>1955</v>
       </c>
+      <c r="D619" t="s">
+        <v>2441</v>
+      </c>
       <c r="E619" t="s">
         <v>1951</v>
       </c>
@@ -27536,6 +28079,9 @@
       <c r="C622" t="s">
         <v>1961</v>
       </c>
+      <c r="D622" t="s">
+        <v>2441</v>
+      </c>
       <c r="E622" t="s">
         <v>1951</v>
       </c>
@@ -27565,6 +28111,9 @@
       <c r="C623" t="s">
         <v>1963</v>
       </c>
+      <c r="D623" t="s">
+        <v>2441</v>
+      </c>
       <c r="E623" t="s">
         <v>1951</v>
       </c>
@@ -27594,6 +28143,9 @@
       <c r="C624" t="s">
         <v>1966</v>
       </c>
+      <c r="D624" t="s">
+        <v>2441</v>
+      </c>
       <c r="E624" t="s">
         <v>1951</v>
       </c>
@@ -27655,6 +28207,9 @@
       <c r="C626" t="s">
         <v>1969</v>
       </c>
+      <c r="D626" t="s">
+        <v>2441</v>
+      </c>
       <c r="E626" t="s">
         <v>1951</v>
       </c>
@@ -27748,6 +28303,9 @@
       <c r="C629" t="s">
         <v>1977</v>
       </c>
+      <c r="D629" t="s">
+        <v>2441</v>
+      </c>
       <c r="E629" t="s">
         <v>1951</v>
       </c>
@@ -27841,6 +28399,9 @@
       <c r="C632" t="s">
         <v>1982</v>
       </c>
+      <c r="D632" t="s">
+        <v>2441</v>
+      </c>
       <c r="E632" t="s">
         <v>216</v>
       </c>
@@ -27902,6 +28463,9 @@
       <c r="C634" t="s">
         <v>1990</v>
       </c>
+      <c r="D634" t="s">
+        <v>2441</v>
+      </c>
       <c r="E634" t="s">
         <v>216</v>
       </c>
@@ -27963,6 +28527,9 @@
       <c r="C636" t="s">
         <v>1997</v>
       </c>
+      <c r="D636" t="s">
+        <v>2441</v>
+      </c>
       <c r="E636" t="s">
         <v>1996</v>
       </c>
@@ -28152,6 +28719,9 @@
       <c r="C642" t="s">
         <v>2011</v>
       </c>
+      <c r="D642" t="s">
+        <v>2441</v>
+      </c>
       <c r="E642" t="s">
         <v>2008</v>
       </c>
@@ -28277,6 +28847,9 @@
       <c r="C646" t="s">
         <v>2020</v>
       </c>
+      <c r="D646" t="s">
+        <v>2441</v>
+      </c>
       <c r="E646" t="s">
         <v>2008</v>
       </c>
@@ -28498,6 +29071,9 @@
       <c r="C653" t="s">
         <v>2040</v>
       </c>
+      <c r="D653" t="s">
+        <v>2441</v>
+      </c>
       <c r="E653" t="s">
         <v>2008</v>
       </c>
@@ -28591,6 +29167,9 @@
       <c r="C656" t="s">
         <v>2048</v>
       </c>
+      <c r="D656" t="s">
+        <v>2441</v>
+      </c>
       <c r="E656" t="s">
         <v>2045</v>
       </c>
@@ -28652,6 +29231,9 @@
       <c r="C658" t="s">
         <v>2052</v>
       </c>
+      <c r="D658" t="s">
+        <v>2441</v>
+      </c>
       <c r="E658" t="s">
         <v>2045</v>
       </c>
@@ -28841,6 +29423,9 @@
       <c r="C664" t="s">
         <v>2068</v>
       </c>
+      <c r="D664" t="s">
+        <v>2441</v>
+      </c>
       <c r="E664" t="s">
         <v>2045</v>
       </c>
@@ -28902,6 +29487,9 @@
       <c r="C666" t="s">
         <v>2074</v>
       </c>
+      <c r="D666" t="s">
+        <v>2441</v>
+      </c>
       <c r="E666" t="s">
         <v>2045</v>
       </c>
@@ -29059,6 +29647,9 @@
       <c r="C671" t="s">
         <v>2084</v>
       </c>
+      <c r="D671" t="s">
+        <v>2441</v>
+      </c>
       <c r="E671" t="s">
         <v>183</v>
       </c>
@@ -29120,6 +29711,9 @@
       <c r="C673" t="s">
         <v>2088</v>
       </c>
+      <c r="D673" t="s">
+        <v>2441</v>
+      </c>
       <c r="E673" t="s">
         <v>183</v>
       </c>
@@ -29277,6 +29871,9 @@
       <c r="C678" t="s">
         <v>2102</v>
       </c>
+      <c r="D678" t="s">
+        <v>2441</v>
+      </c>
       <c r="E678" t="s">
         <v>2095</v>
       </c>
@@ -29306,6 +29903,9 @@
       <c r="C679" t="s">
         <v>2105</v>
       </c>
+      <c r="D679" t="s">
+        <v>2441</v>
+      </c>
       <c r="E679" t="s">
         <v>2095</v>
       </c>
@@ -29367,6 +29967,9 @@
       <c r="C681" t="s">
         <v>2109</v>
       </c>
+      <c r="D681" t="s">
+        <v>2441</v>
+      </c>
       <c r="E681" t="s">
         <v>2095</v>
       </c>
@@ -29460,6 +30063,9 @@
       <c r="C684" t="s">
         <v>2116</v>
       </c>
+      <c r="D684" t="s">
+        <v>2441</v>
+      </c>
       <c r="E684" t="s">
         <v>2095</v>
       </c>
@@ -29585,6 +30191,9 @@
       <c r="C688" t="s">
         <v>2122</v>
       </c>
+      <c r="D688" t="s">
+        <v>2441</v>
+      </c>
       <c r="E688" t="s">
         <v>2095</v>
       </c>
@@ -29742,6 +30351,9 @@
       <c r="C693" t="s">
         <v>2136</v>
       </c>
+      <c r="D693" t="s">
+        <v>2441</v>
+      </c>
       <c r="E693" t="s">
         <v>2132</v>
       </c>
@@ -29867,6 +30479,9 @@
       <c r="C697" t="s">
         <v>2145</v>
       </c>
+      <c r="D697" t="s">
+        <v>2441</v>
+      </c>
       <c r="E697" t="s">
         <v>2132</v>
       </c>
@@ -30056,6 +30671,9 @@
       <c r="C703" t="s">
         <v>2158</v>
       </c>
+      <c r="D703" t="s">
+        <v>2441</v>
+      </c>
       <c r="E703" t="s">
         <v>2132</v>
       </c>
@@ -30117,6 +30735,9 @@
       <c r="C705" t="s">
         <v>2162</v>
       </c>
+      <c r="D705" t="s">
+        <v>2441</v>
+      </c>
       <c r="E705" t="s">
         <v>2163</v>
       </c>
@@ -30146,6 +30767,9 @@
       <c r="C706" t="s">
         <v>2164</v>
       </c>
+      <c r="D706" t="s">
+        <v>2441</v>
+      </c>
       <c r="E706" t="s">
         <v>2163</v>
       </c>
@@ -30207,6 +30831,9 @@
       <c r="C708" t="s">
         <v>2170</v>
       </c>
+      <c r="D708" t="s">
+        <v>2441</v>
+      </c>
       <c r="E708" t="s">
         <v>2163</v>
       </c>
@@ -30236,6 +30863,9 @@
       <c r="C709" t="s">
         <v>2173</v>
       </c>
+      <c r="D709" t="s">
+        <v>2441</v>
+      </c>
       <c r="E709" t="s">
         <v>2163</v>
       </c>
@@ -30265,6 +30895,9 @@
       <c r="C710" t="s">
         <v>2174</v>
       </c>
+      <c r="D710" t="s">
+        <v>2441</v>
+      </c>
       <c r="E710" t="s">
         <v>2163</v>
       </c>
@@ -30326,6 +30959,9 @@
       <c r="C712" t="s">
         <v>2177</v>
       </c>
+      <c r="D712" t="s">
+        <v>2441</v>
+      </c>
       <c r="E712" t="s">
         <v>2163</v>
       </c>
@@ -30675,6 +31311,9 @@
       <c r="C723" t="s">
         <v>2203</v>
       </c>
+      <c r="D723" t="s">
+        <v>2441</v>
+      </c>
       <c r="E723" t="s">
         <v>2186</v>
       </c>
@@ -30704,6 +31343,9 @@
       <c r="C724" t="s">
         <v>2206</v>
       </c>
+      <c r="D724" t="s">
+        <v>2441</v>
+      </c>
       <c r="E724" t="s">
         <v>2186</v>
       </c>
@@ -30829,6 +31471,9 @@
       <c r="C728" t="s">
         <v>2214</v>
       </c>
+      <c r="D728" t="s">
+        <v>2441</v>
+      </c>
       <c r="E728" t="s">
         <v>2186</v>
       </c>
@@ -30858,6 +31503,9 @@
       <c r="C729" t="s">
         <v>2217</v>
       </c>
+      <c r="D729" t="s">
+        <v>2441</v>
+      </c>
       <c r="E729" t="s">
         <v>2218</v>
       </c>
@@ -31015,6 +31663,9 @@
       <c r="C734" t="s">
         <v>2230</v>
       </c>
+      <c r="D734" t="s">
+        <v>2441</v>
+      </c>
       <c r="E734" t="s">
         <v>2218</v>
       </c>
@@ -31140,6 +31791,9 @@
       <c r="C738" t="s">
         <v>2239</v>
       </c>
+      <c r="D738" t="s">
+        <v>2441</v>
+      </c>
       <c r="E738" t="s">
         <v>2240</v>
       </c>
@@ -31169,6 +31823,9 @@
       <c r="C739" t="s">
         <v>2242</v>
       </c>
+      <c r="D739" t="s">
+        <v>2441</v>
+      </c>
       <c r="E739" t="s">
         <v>2240</v>
       </c>
@@ -31294,6 +31951,9 @@
       <c r="C743" t="s">
         <v>2252</v>
       </c>
+      <c r="D743" t="s">
+        <v>2441</v>
+      </c>
       <c r="E743" t="s">
         <v>2240</v>
       </c>
@@ -31579,6 +32239,9 @@
       <c r="C752" t="s">
         <v>2274</v>
       </c>
+      <c r="D752" t="s">
+        <v>2441</v>
+      </c>
       <c r="E752" t="s">
         <v>2240</v>
       </c>
@@ -31640,6 +32303,9 @@
       <c r="C754" t="s">
         <v>2277</v>
       </c>
+      <c r="D754" t="s">
+        <v>2441</v>
+      </c>
       <c r="E754" t="s">
         <v>2278</v>
       </c>
@@ -31765,6 +32431,9 @@
       <c r="C758" t="s">
         <v>2286</v>
       </c>
+      <c r="D758" t="s">
+        <v>2441</v>
+      </c>
       <c r="E758" t="s">
         <v>2278</v>
       </c>
@@ -31794,6 +32463,9 @@
       <c r="C759" t="s">
         <v>2288</v>
       </c>
+      <c r="D759" t="s">
+        <v>2441</v>
+      </c>
       <c r="E759" t="s">
         <v>2278</v>
       </c>
@@ -31823,6 +32495,9 @@
       <c r="C760" t="s">
         <v>2290</v>
       </c>
+      <c r="D760" t="s">
+        <v>2441</v>
+      </c>
       <c r="E760" t="s">
         <v>2278</v>
       </c>
@@ -31852,6 +32527,9 @@
       <c r="C761" t="s">
         <v>2292</v>
       </c>
+      <c r="D761" t="s">
+        <v>2441</v>
+      </c>
       <c r="E761" t="s">
         <v>2278</v>
       </c>
@@ -32137,6 +32815,9 @@
       <c r="C770" t="s">
         <v>2314</v>
       </c>
+      <c r="D770" t="s">
+        <v>2441</v>
+      </c>
       <c r="E770" t="s">
         <v>2309</v>
       </c>
@@ -32166,6 +32847,9 @@
       <c r="C771" t="s">
         <v>2316</v>
       </c>
+      <c r="D771" t="s">
+        <v>2441</v>
+      </c>
       <c r="E771" t="s">
         <v>2309</v>
       </c>
@@ -32195,6 +32879,9 @@
       <c r="C772" t="s">
         <v>2318</v>
       </c>
+      <c r="D772" t="s">
+        <v>2441</v>
+      </c>
       <c r="E772" t="s">
         <v>2309</v>
       </c>
@@ -32416,6 +33103,9 @@
       <c r="C779" t="s">
         <v>2334</v>
       </c>
+      <c r="D779" t="s">
+        <v>2441</v>
+      </c>
       <c r="E779" t="s">
         <v>2309</v>
       </c>
@@ -32733,6 +33423,9 @@
       <c r="C789" t="s">
         <v>2361</v>
       </c>
+      <c r="D789" t="s">
+        <v>2441</v>
+      </c>
       <c r="E789" t="s">
         <v>2357</v>
       </c>
@@ -32826,6 +33519,9 @@
       <c r="C792" t="s">
         <v>2366</v>
       </c>
+      <c r="D792" t="s">
+        <v>2441</v>
+      </c>
       <c r="E792" t="s">
         <v>2357</v>
       </c>
@@ -32983,6 +33679,9 @@
       <c r="C797" t="s">
         <v>2377</v>
       </c>
+      <c r="D797" t="s">
+        <v>2441</v>
+      </c>
       <c r="E797" t="s">
         <v>2357</v>
       </c>
@@ -33140,6 +33839,9 @@
       <c r="C802" t="s">
         <v>2389</v>
       </c>
+      <c r="D802" t="s">
+        <v>2441</v>
+      </c>
       <c r="E802" t="s">
         <v>2357</v>
       </c>
@@ -33201,6 +33903,9 @@
       <c r="C804" t="s">
         <v>2393</v>
       </c>
+      <c r="D804" t="s">
+        <v>2441</v>
+      </c>
       <c r="E804" t="s">
         <v>2394</v>
       </c>
@@ -33262,6 +33967,9 @@
       <c r="C806" t="s">
         <v>2401</v>
       </c>
+      <c r="D806" t="s">
+        <v>2441</v>
+      </c>
       <c r="E806" t="s">
         <v>2394</v>
       </c>
@@ -33387,6 +34095,9 @@
       <c r="C810" t="s">
         <v>2409</v>
       </c>
+      <c r="D810" t="s">
+        <v>2441</v>
+      </c>
       <c r="E810" t="s">
         <v>2394</v>
       </c>
@@ -33448,6 +34159,9 @@
       <c r="C812" t="s">
         <v>2412</v>
       </c>
+      <c r="D812" t="s">
+        <v>2441</v>
+      </c>
       <c r="E812" t="s">
         <v>2394</v>
       </c>
@@ -33477,6 +34191,9 @@
       <c r="C813" t="s">
         <v>2413</v>
       </c>
+      <c r="D813" t="s">
+        <v>2441</v>
+      </c>
       <c r="E813" t="s">
         <v>2414</v>
       </c>
@@ -33506,6 +34223,9 @@
       <c r="C814" t="s">
         <v>2416</v>
       </c>
+      <c r="D814" t="s">
+        <v>2441</v>
+      </c>
       <c r="E814" t="s">
         <v>2414</v>
       </c>
@@ -33535,6 +34255,9 @@
       <c r="C815" t="s">
         <v>2418</v>
       </c>
+      <c r="D815" t="s">
+        <v>2441</v>
+      </c>
       <c r="E815" t="s">
         <v>2414</v>
       </c>
@@ -33596,6 +34319,9 @@
       <c r="C817" t="s">
         <v>2422</v>
       </c>
+      <c r="D817" t="s">
+        <v>2441</v>
+      </c>
       <c r="E817" t="s">
         <v>2414</v>
       </c>
@@ -33689,6 +34415,9 @@
       <c r="C820" t="s">
         <v>2428</v>
       </c>
+      <c r="D820" t="s">
+        <v>2441</v>
+      </c>
       <c r="E820" t="s">
         <v>2414</v>
       </c>
@@ -33718,6 +34447,9 @@
       <c r="C821" t="s">
         <v>2430</v>
       </c>
+      <c r="D821" t="s">
+        <v>2441</v>
+      </c>
       <c r="E821" t="s">
         <v>2414</v>
       </c>
@@ -33747,6 +34479,9 @@
       <c r="C822" t="s">
         <v>2433</v>
       </c>
+      <c r="D822" t="s">
+        <v>2441</v>
+      </c>
       <c r="E822" t="s">
         <v>2414</v>
       </c>
@@ -33776,6 +34511,9 @@
       <c r="C823" t="s">
         <v>2436</v>
       </c>
+      <c r="D823" t="s">
+        <v>2441</v>
+      </c>
       <c r="E823" t="s">
         <v>2414</v>
       </c>
@@ -33837,6 +34575,9 @@
       <c r="C825" t="s">
         <v>2377</v>
       </c>
+      <c r="D825" t="s">
+        <v>2441</v>
+      </c>
       <c r="E825" t="s">
         <v>2357</v>
       </c>
@@ -33897,6 +34638,9 @@
       </c>
       <c r="C827" t="s">
         <v>2412</v>
+      </c>
+      <c r="D827" t="s">
+        <v>2441</v>
       </c>
       <c r="E827" t="s">
         <v>2394</v>

</xml_diff>